<commit_message>
Lex + file delete, Syn + action table
</commit_message>
<xml_diff>
--- a/SyntaxAnalyzer/table.xlsx
+++ b/SyntaxAnalyzer/table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="580" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -686,8 +686,14 @@
       <scheme val="minor"/>
       <color theme="1"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,156 +705,193 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.150000"/>
+        <bgColor theme="0" tint="-0.150000"/>
       </patternFill>
     </fill>
     <fill>
@@ -858,15 +901,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -881,33 +922,25 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -922,9 +955,7 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -939,9 +970,7 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -956,17 +985,13 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <top style="thin">
@@ -975,14 +1000,10 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <top style="thin">
@@ -991,6 +1012,23 @@
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
       <diagonal style="none">
         <color rgb="FF000000"/>
       </diagonal>
@@ -1057,7 +1095,7 @@
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1072,6 +1110,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1130,7 +1171,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A3:AK87" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A2:AK86" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="37">
     <tableColumn id="1" name="열1" totalsRowLabel="요약"/>
     <tableColumn id="2" name="열2"/>
@@ -1471,11 +1512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK87"/>
+  <dimension ref="A1:AK86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V87" sqref="V87"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1597,10 +1638,59 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:37"/>
+    <row r="2" spans="1:37">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="W2" s="3">
+        <v>85</v>
+      </c>
+      <c r="X2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+    </row>
     <row r="3" spans="1:37">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>36</v>
@@ -1628,7 +1718,7 @@
         <v>88</v>
       </c>
       <c r="W3" s="3">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="X3" s="3">
         <v>2</v>
@@ -1650,11 +1740,9 @@
     </row>
     <row r="4" spans="1:37">
       <c r="A4" s="0">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1675,17 +1763,11 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="W4" s="3">
-        <v>3</v>
-      </c>
-      <c r="X4" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>4</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
@@ -1700,9 +1782,11 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="0">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1723,11 +1807,17 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="W5" s="3">
+        <v>5</v>
+      </c>
+      <c r="X5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>4</v>
+      </c>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -1742,11 +1832,9 @@
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="0">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1767,17 +1855,11 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="W6" s="3">
-        <v>5</v>
-      </c>
-      <c r="X6" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>4</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
@@ -1792,13 +1874,15 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1814,9 +1898,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
@@ -1824,7 +1906,9 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
+      <c r="AD7" s="3">
+        <v>7</v>
+      </c>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
@@ -1834,15 +1918,13 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1852,7 +1934,9 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="P8" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -1866,9 +1950,7 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="3">
-        <v>7</v>
-      </c>
+      <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
@@ -1878,31 +1960,43 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="0">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+      <c r="U9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
@@ -1920,43 +2014,35 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="0">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="R10" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
@@ -1974,35 +2060,43 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="0">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+      <c r="U11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
@@ -2020,28 +2114,20 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -2049,18 +2135,18 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="S12" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="T12" s="3"/>
-      <c r="U12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
+      <c r="Z12" s="3">
+        <v>19</v>
+      </c>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
@@ -2074,15 +2160,15 @@
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="0">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2095,18 +2181,14 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="3">
-        <v>19</v>
-      </c>
+      <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
@@ -2120,15 +2202,13 @@
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2139,9 +2219,13 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="Q14" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="S14" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -2149,7 +2233,9 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
+      <c r="AA14" s="3">
+        <v>14</v>
+      </c>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
@@ -2162,9 +2248,8 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="0">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>14</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2179,12 +2264,10 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -2193,9 +2276,7 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="3">
-        <v>14</v>
-      </c>
+      <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
@@ -2208,12 +2289,14 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="0">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -2226,9 +2309,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -2249,14 +2330,15 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="0">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -2290,15 +2372,13 @@
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -2309,9 +2389,13 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="Q18" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="S18" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -2319,7 +2403,9 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
+      <c r="AA18" s="3">
+        <v>18</v>
+      </c>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
@@ -2332,7 +2418,7 @@
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2349,12 +2435,10 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
@@ -2363,9 +2447,7 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="3">
-        <v>18</v>
-      </c>
+      <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
@@ -2378,7 +2460,7 @@
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2398,7 +2480,7 @@
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -2420,7 +2502,7 @@
     </row>
     <row r="21" spans="1:36">
       <c r="A21" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2439,10 +2521,10 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
-      <c r="S21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
@@ -2462,18 +2544,30 @@
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="0">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -2481,20 +2575,27 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
+      <c r="X22" s="3">
+        <v>24</v>
+      </c>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
+      <c r="AB22" s="3">
+        <v>45</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>25</v>
+      </c>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
@@ -2504,30 +2605,20 @@
     </row>
     <row r="23" spans="1:36">
       <c r="A23" s="0">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -2535,26 +2626,19 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
-      <c r="X23" s="3">
-        <v>24</v>
-      </c>
+      <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="3">
-        <v>45</v>
-      </c>
-      <c r="AC23" s="3">
-        <v>30</v>
-      </c>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
       <c r="AD23" s="3">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
@@ -2565,15 +2649,13 @@
     </row>
     <row r="24" spans="1:36">
       <c r="A24" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -2581,9 +2663,13 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="N24" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
@@ -2597,9 +2683,7 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
-      <c r="AD24" s="3">
-        <v>7</v>
-      </c>
+      <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
@@ -2609,32 +2693,42 @@
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="0">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
+      <c r="U25" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -2653,42 +2747,30 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" s="0">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="P26" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -2707,30 +2789,42 @@
     </row>
     <row r="27" spans="1:36">
       <c r="A27" s="0">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
+      <c r="U27" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -2749,42 +2843,30 @@
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="0">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>142</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
-      <c r="U28" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -2803,7 +2885,7 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2817,13 +2899,13 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
+      <c r="R29" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
@@ -2845,13 +2927,19 @@
     </row>
     <row r="30" spans="1:36">
       <c r="A30" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2864,7 +2952,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -2881,87 +2969,91 @@
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
-      <c r="AH30" s="3"/>
-      <c r="AI30" s="3"/>
+      <c r="AH30" s="3">
+        <v>42</v>
+      </c>
+      <c r="AI30" s="3">
+        <v>32</v>
+      </c>
       <c r="AJ30" s="3"/>
     </row>
     <row r="31" spans="1:36">
       <c r="A31" s="0">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="I31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
-      <c r="R31" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
+      <c r="U31" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
+      <c r="X31" s="3">
+        <v>24</v>
+      </c>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
+      <c r="AB31" s="3">
+        <v>31</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>25</v>
+      </c>
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
-      <c r="AH31" s="3">
-        <v>42</v>
-      </c>
-      <c r="AI31" s="3">
-        <v>32</v>
-      </c>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
     </row>
     <row r="32" spans="1:36">
       <c r="A32" s="0">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2973,25 +3065,17 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
-      <c r="X32" s="3">
-        <v>24</v>
-      </c>
+      <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
-      <c r="AB32" s="3">
-        <v>31</v>
-      </c>
-      <c r="AC32" s="3">
-        <v>30</v>
-      </c>
-      <c r="AD32" s="3">
-        <v>25</v>
-      </c>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
@@ -3001,7 +3085,7 @@
     </row>
     <row r="33" spans="1:37">
       <c r="A33" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3012,9 +3096,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -3022,11 +3104,11 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
+      <c r="S33" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="T33" s="3"/>
-      <c r="U33" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -3045,7 +3127,7 @@
     </row>
     <row r="34" spans="1:37">
       <c r="A34" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3064,10 +3146,10 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="T34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
@@ -3087,18 +3169,30 @@
     </row>
     <row r="35" spans="1:37">
       <c r="A35" s="0">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="I35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -3107,19 +3201,27 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="U35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
+      <c r="X35" s="3">
+        <v>24</v>
+      </c>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
-      <c r="AB35" s="3"/>
-      <c r="AC35" s="3"/>
-      <c r="AD35" s="3"/>
+      <c r="AB35" s="3">
+        <v>35</v>
+      </c>
+      <c r="AC35" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD35" s="3">
+        <v>25</v>
+      </c>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
@@ -3129,30 +3231,18 @@
     </row>
     <row r="36" spans="1:37">
       <c r="A36" s="0">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -3163,25 +3253,17 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3" t="s">
-        <v>140</v>
+        <v>63</v>
       </c>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
-      <c r="X36" s="3">
-        <v>24</v>
-      </c>
+      <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
-      <c r="AB36" s="3">
-        <v>35</v>
-      </c>
-      <c r="AC36" s="3">
-        <v>30</v>
-      </c>
-      <c r="AD36" s="3">
-        <v>25</v>
-      </c>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
@@ -3191,18 +3273,32 @@
     </row>
     <row r="37" spans="1:37">
       <c r="A37" s="0">
-        <v>35</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -3213,7 +3309,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
@@ -3230,34 +3326,35 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
+      <c r="AK37" s="0">
+        <v>37</v>
+      </c>
     </row>
     <row r="38" spans="1:37">
       <c r="A38" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H38" s="3"/>
       <c r="I38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -3269,7 +3366,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
@@ -3286,36 +3383,21 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
-      <c r="AK38" s="0">
-        <v>37</v>
-      </c>
     </row>
     <row r="39" spans="1:37">
       <c r="A39" s="0">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>145</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -3324,10 +3406,10 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="T39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
@@ -3346,18 +3428,30 @@
     </row>
     <row r="40" spans="1:37">
       <c r="A40" s="0">
-        <v>38</v>
-      </c>
-      <c r="B40" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="I40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3366,19 +3460,27 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
-      <c r="T40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
+      <c r="X40" s="3">
+        <v>24</v>
+      </c>
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
+      <c r="AB40" s="3">
+        <v>40</v>
+      </c>
+      <c r="AC40" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD40" s="3">
+        <v>25</v>
+      </c>
       <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
@@ -3388,30 +3490,18 @@
     </row>
     <row r="41" spans="1:37">
       <c r="A41" s="0">
-        <v>39</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -3422,25 +3512,17 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
-      <c r="X41" s="3">
-        <v>24</v>
-      </c>
+      <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
-      <c r="AB41" s="3">
-        <v>40</v>
-      </c>
-      <c r="AC41" s="3">
-        <v>30</v>
-      </c>
-      <c r="AD41" s="3">
-        <v>25</v>
-      </c>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
       <c r="AF41" s="3"/>
       <c r="AG41" s="3"/>
@@ -3450,18 +3532,30 @@
     </row>
     <row r="42" spans="1:37">
       <c r="A42" s="0">
-        <v>40</v>
-      </c>
-      <c r="B42" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="I42" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -3472,7 +3566,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
@@ -3492,42 +3586,30 @@
     </row>
     <row r="43" spans="1:37">
       <c r="A43" s="0">
-        <v>41</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>146</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
+      <c r="O43" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
-      <c r="U43" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="U43" s="3"/>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
@@ -3546,13 +3628,19 @@
     </row>
     <row r="44" spans="1:37">
       <c r="A44" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3561,12 +3649,12 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
+      <c r="R44" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
@@ -3582,25 +3670,21 @@
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
-      <c r="AH44" s="3"/>
+      <c r="AH44" s="3">
+        <v>44</v>
+      </c>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
     </row>
     <row r="45" spans="1:37">
       <c r="A45" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3610,12 +3694,14 @@
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="Q45" s="3"/>
-      <c r="R45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
@@ -3630,15 +3716,13 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
-      <c r="AH45" s="3">
-        <v>44</v>
-      </c>
+      <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
     </row>
     <row r="46" spans="1:37">
       <c r="A46" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3649,19 +3733,17 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="K46" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
-      <c r="S46" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="S46" s="3"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -3678,11 +3760,13 @@
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
-      <c r="AJ46" s="3"/>
+      <c r="AJ46" s="3">
+        <v>46</v>
+      </c>
     </row>
     <row r="47" spans="1:37">
       <c r="A47" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3693,9 +3777,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -3705,7 +3787,9 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
+      <c r="U47" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
@@ -3720,15 +3804,15 @@
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
-      <c r="AJ47" s="3">
-        <v>46</v>
-      </c>
+      <c r="AJ47" s="3"/>
     </row>
     <row r="48" spans="1:37">
       <c r="A48" s="0">
-        <v>46</v>
-      </c>
-      <c r="B48" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -3747,10 +3831,10 @@
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
-      <c r="U48" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="V48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
@@ -3768,13 +3852,19 @@
     </row>
     <row r="49" spans="1:36">
       <c r="A49" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="C49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -3786,13 +3876,13 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
+      <c r="R49" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
-      <c r="V49" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
@@ -3804,25 +3894,21 @@
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
-      <c r="AH49" s="3"/>
+      <c r="AH49" s="3">
+        <v>49</v>
+      </c>
       <c r="AI49" s="3"/>
       <c r="AJ49" s="3"/>
     </row>
     <row r="50" spans="1:36">
       <c r="A50" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -3832,11 +3918,11 @@
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
+      <c r="P50" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="Q50" s="3"/>
-      <c r="R50" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
@@ -3852,15 +3938,13 @@
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
       <c r="AG50" s="3"/>
-      <c r="AH50" s="3">
-        <v>49</v>
-      </c>
+      <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
       <c r="AJ50" s="3"/>
     </row>
     <row r="51" spans="1:36">
       <c r="A51" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -3876,14 +3960,14 @@
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
-      <c r="P51" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
+      <c r="U51" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
@@ -3902,7 +3986,7 @@
     </row>
     <row r="52" spans="1:36">
       <c r="A52" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -3920,12 +4004,12 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
+      <c r="R52" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
-      <c r="U52" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="U52" s="3"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
@@ -3944,13 +4028,19 @@
     </row>
     <row r="53" spans="1:36">
       <c r="A53" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -3963,7 +4053,7 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
@@ -3980,25 +4070,23 @@
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
       <c r="AG53" s="3"/>
-      <c r="AH53" s="3"/>
-      <c r="AI53" s="3"/>
+      <c r="AH53" s="3">
+        <v>42</v>
+      </c>
+      <c r="AI53" s="3">
+        <v>53</v>
+      </c>
       <c r="AJ53" s="3"/>
     </row>
     <row r="54" spans="1:36">
       <c r="A54" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -4010,10 +4098,10 @@
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
-      <c r="R54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
@@ -4028,17 +4116,13 @@
       <c r="AE54" s="3"/>
       <c r="AF54" s="3"/>
       <c r="AG54" s="3"/>
-      <c r="AH54" s="3">
-        <v>42</v>
-      </c>
-      <c r="AI54" s="3">
-        <v>53</v>
-      </c>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
       <c r="AJ54" s="3"/>
     </row>
     <row r="55" spans="1:36">
       <c r="A55" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4057,10 +4141,10 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
-      <c r="S55" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="T55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
@@ -4080,18 +4164,30 @@
     </row>
     <row r="56" spans="1:36">
       <c r="A56" s="0">
-        <v>54</v>
-      </c>
-      <c r="B56" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
@@ -4100,19 +4196,27 @@
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
-      <c r="T56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="U56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
-      <c r="X56" s="3"/>
+      <c r="X56" s="3">
+        <v>24</v>
+      </c>
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
       <c r="AA56" s="3"/>
-      <c r="AB56" s="3"/>
-      <c r="AC56" s="3"/>
-      <c r="AD56" s="3"/>
+      <c r="AB56" s="3">
+        <v>56</v>
+      </c>
+      <c r="AC56" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD56" s="3">
+        <v>25</v>
+      </c>
       <c r="AE56" s="3"/>
       <c r="AF56" s="3"/>
       <c r="AG56" s="3"/>
@@ -4122,30 +4226,18 @@
     </row>
     <row r="57" spans="1:36">
       <c r="A57" s="0">
-        <v>55</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
@@ -4156,25 +4248,17 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
       <c r="U57" s="3" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="V57" s="3"/>
       <c r="W57" s="3"/>
-      <c r="X57" s="3">
-        <v>24</v>
-      </c>
+      <c r="X57" s="3"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
       <c r="AA57" s="3"/>
-      <c r="AB57" s="3">
-        <v>56</v>
-      </c>
-      <c r="AC57" s="3">
-        <v>30</v>
-      </c>
-      <c r="AD57" s="3">
-        <v>25</v>
-      </c>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
       <c r="AE57" s="3"/>
       <c r="AF57" s="3"/>
       <c r="AG57" s="3"/>
@@ -4184,18 +4268,30 @@
     </row>
     <row r="58" spans="1:36">
       <c r="A58" s="0">
-        <v>56</v>
-      </c>
-      <c r="B58" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
+      <c r="I58" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
@@ -4206,7 +4302,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="V58" s="3"/>
       <c r="W58" s="3"/>
@@ -4226,42 +4322,30 @@
     </row>
     <row r="59" spans="1:36">
       <c r="A59" s="0">
-        <v>57</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>151</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
+      <c r="R59" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
-      <c r="U59" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="U59" s="3"/>
       <c r="V59" s="3"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
@@ -4280,13 +4364,15 @@
     </row>
     <row r="60" spans="1:36">
       <c r="A60" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
@@ -4298,9 +4384,7 @@
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
-      <c r="R60" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="R60" s="3"/>
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
@@ -4312,7 +4396,9 @@
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
       <c r="AC60" s="3"/>
-      <c r="AD60" s="3"/>
+      <c r="AD60" s="3">
+        <v>60</v>
+      </c>
       <c r="AE60" s="3"/>
       <c r="AF60" s="3"/>
       <c r="AG60" s="3"/>
@@ -4322,15 +4408,13 @@
     </row>
     <row r="61" spans="1:36">
       <c r="A61" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -4340,7 +4424,9 @@
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
+      <c r="P61" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="3"/>
@@ -4354,9 +4440,7 @@
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
       <c r="AC61" s="3"/>
-      <c r="AD61" s="3">
-        <v>60</v>
-      </c>
+      <c r="AD61" s="3"/>
       <c r="AE61" s="3"/>
       <c r="AF61" s="3"/>
       <c r="AG61" s="3"/>
@@ -4366,13 +4450,19 @@
     </row>
     <row r="62" spans="1:36">
       <c r="A62" s="0">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -4382,11 +4472,11 @@
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
-      <c r="P62" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
+      <c r="R62" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
@@ -4402,25 +4492,23 @@
       <c r="AE62" s="3"/>
       <c r="AF62" s="3"/>
       <c r="AG62" s="3"/>
-      <c r="AH62" s="3"/>
-      <c r="AI62" s="3"/>
+      <c r="AH62" s="3">
+        <v>42</v>
+      </c>
+      <c r="AI62" s="3">
+        <v>62</v>
+      </c>
       <c r="AJ62" s="3"/>
     </row>
     <row r="63" spans="1:36">
       <c r="A63" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -4430,11 +4518,11 @@
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
+      <c r="P63" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="Q63" s="3"/>
-      <c r="R63" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="R63" s="3"/>
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
@@ -4450,17 +4538,13 @@
       <c r="AE63" s="3"/>
       <c r="AF63" s="3"/>
       <c r="AG63" s="3"/>
-      <c r="AH63" s="3">
-        <v>42</v>
-      </c>
-      <c r="AI63" s="3">
-        <v>62</v>
-      </c>
+      <c r="AH63" s="3"/>
+      <c r="AI63" s="3"/>
       <c r="AJ63" s="3"/>
     </row>
     <row r="64" spans="1:36">
       <c r="A64" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4476,9 +4560,7 @@
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
-      <c r="P64" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
       <c r="S64" s="3"/>
@@ -4492,7 +4574,9 @@
       <c r="AA64" s="3"/>
       <c r="AB64" s="3"/>
       <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
+      <c r="AD64" s="3">
+        <v>64</v>
+      </c>
       <c r="AE64" s="3"/>
       <c r="AF64" s="3"/>
       <c r="AG64" s="3"/>
@@ -4502,7 +4586,7 @@
     </row>
     <row r="65" spans="1:36">
       <c r="A65" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -4521,7 +4605,9 @@
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
+      <c r="S65" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="T65" s="3"/>
       <c r="U65" s="3"/>
       <c r="V65" s="3"/>
@@ -4532,9 +4618,7 @@
       <c r="AA65" s="3"/>
       <c r="AB65" s="3"/>
       <c r="AC65" s="3"/>
-      <c r="AD65" s="3">
-        <v>64</v>
-      </c>
+      <c r="AD65" s="3"/>
       <c r="AE65" s="3"/>
       <c r="AF65" s="3"/>
       <c r="AG65" s="3"/>
@@ -4544,7 +4628,7 @@
     </row>
     <row r="66" spans="1:36">
       <c r="A66" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4563,10 +4647,10 @@
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
-      <c r="S66" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="T66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
       <c r="W66" s="3"/>
@@ -4586,18 +4670,30 @@
     </row>
     <row r="67" spans="1:36">
       <c r="A67" s="0">
-        <v>65</v>
-      </c>
-      <c r="B67" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
+      <c r="I67" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
@@ -4606,19 +4702,27 @@
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
       <c r="S67" s="3"/>
-      <c r="T67" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="U67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="V67" s="3"/>
       <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
+      <c r="X67" s="3">
+        <v>24</v>
+      </c>
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
       <c r="AA67" s="3"/>
-      <c r="AB67" s="3"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
+      <c r="AB67" s="3">
+        <v>67</v>
+      </c>
+      <c r="AC67" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD67" s="3">
+        <v>25</v>
+      </c>
       <c r="AE67" s="3"/>
       <c r="AF67" s="3"/>
       <c r="AG67" s="3"/>
@@ -4628,30 +4732,18 @@
     </row>
     <row r="68" spans="1:36">
       <c r="A68" s="0">
-        <v>66</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
@@ -4662,25 +4754,17 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
       <c r="U68" s="3" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="V68" s="3"/>
       <c r="W68" s="3"/>
-      <c r="X68" s="3">
-        <v>24</v>
-      </c>
+      <c r="X68" s="3"/>
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
       <c r="AA68" s="3"/>
-      <c r="AB68" s="3">
-        <v>67</v>
-      </c>
-      <c r="AC68" s="3">
-        <v>30</v>
-      </c>
-      <c r="AD68" s="3">
-        <v>25</v>
-      </c>
+      <c r="AB68" s="3"/>
+      <c r="AC68" s="3"/>
+      <c r="AD68" s="3"/>
       <c r="AE68" s="3"/>
       <c r="AF68" s="3"/>
       <c r="AG68" s="3"/>
@@ -4690,18 +4774,30 @@
     </row>
     <row r="69" spans="1:36">
       <c r="A69" s="0">
-        <v>67</v>
-      </c>
-      <c r="B69" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
+      <c r="I69" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
@@ -4712,7 +4808,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
       <c r="U69" s="3" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="V69" s="3"/>
       <c r="W69" s="3"/>
@@ -4732,42 +4828,38 @@
     </row>
     <row r="70" spans="1:36">
       <c r="A70" s="0">
-        <v>68</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="F70" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>152</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
+      <c r="R70" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
-      <c r="U70" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="U70" s="3"/>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
@@ -4777,30 +4869,30 @@
       <c r="AB70" s="3"/>
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
-      <c r="AE70" s="3"/>
-      <c r="AF70" s="3"/>
-      <c r="AG70" s="3"/>
-      <c r="AH70" s="3"/>
+      <c r="AE70" s="3">
+        <v>70</v>
+      </c>
+      <c r="AF70" s="3">
+        <v>72</v>
+      </c>
+      <c r="AG70" s="3">
+        <v>74</v>
+      </c>
+      <c r="AH70" s="3">
+        <v>80</v>
+      </c>
       <c r="AI70" s="3"/>
       <c r="AJ70" s="3"/>
     </row>
     <row r="71" spans="1:36">
       <c r="A71" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -4810,12 +4902,14 @@
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
+      <c r="P71" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="Q71" s="3"/>
-      <c r="R71" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="T71" s="3"/>
       <c r="U71" s="3"/>
       <c r="V71" s="3"/>
@@ -4827,24 +4921,16 @@
       <c r="AB71" s="3"/>
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
-      <c r="AE71" s="3">
-        <v>70</v>
-      </c>
-      <c r="AF71" s="3">
-        <v>72</v>
-      </c>
-      <c r="AG71" s="3">
-        <v>74</v>
-      </c>
-      <c r="AH71" s="3">
-        <v>80</v>
-      </c>
+      <c r="AE71" s="3"/>
+      <c r="AF71" s="3"/>
+      <c r="AG71" s="3"/>
+      <c r="AH71" s="3"/>
       <c r="AI71" s="3"/>
       <c r="AJ71" s="3"/>
     </row>
     <row r="72" spans="1:36">
       <c r="A72" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4861,12 +4947,12 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
       <c r="S72" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
@@ -4888,7 +4974,7 @@
     </row>
     <row r="73" spans="1:36">
       <c r="A73" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4905,12 +4991,12 @@
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
       <c r="S73" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="T73" s="3"/>
       <c r="U73" s="3"/>
@@ -4932,13 +5018,19 @@
     </row>
     <row r="74" spans="1:36">
       <c r="A74" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -4948,14 +5040,12 @@
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
-      <c r="P74" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
-      <c r="R74" s="3"/>
-      <c r="S74" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="R74" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S74" s="3"/>
       <c r="T74" s="3"/>
       <c r="U74" s="3"/>
       <c r="V74" s="3"/>
@@ -4969,41 +5059,43 @@
       <c r="AD74" s="3"/>
       <c r="AE74" s="3"/>
       <c r="AF74" s="3"/>
-      <c r="AG74" s="3"/>
-      <c r="AH74" s="3"/>
+      <c r="AG74" s="3">
+        <v>84</v>
+      </c>
+      <c r="AH74" s="3">
+        <v>80</v>
+      </c>
       <c r="AI74" s="3"/>
       <c r="AJ74" s="3"/>
     </row>
     <row r="75" spans="1:36">
       <c r="A75" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3"/>
-      <c r="C75" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
+      <c r="L75" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
+      <c r="P75" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="Q75" s="3"/>
-      <c r="R75" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="T75" s="3"/>
       <c r="U75" s="3"/>
       <c r="V75" s="3"/>
@@ -5017,43 +5109,41 @@
       <c r="AD75" s="3"/>
       <c r="AE75" s="3"/>
       <c r="AF75" s="3"/>
-      <c r="AG75" s="3">
-        <v>84</v>
-      </c>
-      <c r="AH75" s="3">
-        <v>80</v>
-      </c>
+      <c r="AG75" s="3"/>
+      <c r="AH75" s="3"/>
       <c r="AI75" s="3"/>
       <c r="AJ75" s="3"/>
     </row>
     <row r="76" spans="1:36">
       <c r="A76" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
-      <c r="L76" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="L76" s="3"/>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
-      <c r="P76" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
-      <c r="R76" s="3"/>
-      <c r="S76" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="R76" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S76" s="3"/>
       <c r="T76" s="3"/>
       <c r="U76" s="3"/>
       <c r="V76" s="3"/>
@@ -5066,27 +5156,27 @@
       <c r="AC76" s="3"/>
       <c r="AD76" s="3"/>
       <c r="AE76" s="3"/>
-      <c r="AF76" s="3"/>
-      <c r="AG76" s="3"/>
-      <c r="AH76" s="3"/>
+      <c r="AF76" s="3">
+        <v>76</v>
+      </c>
+      <c r="AG76" s="3">
+        <v>74</v>
+      </c>
+      <c r="AH76" s="3">
+        <v>80</v>
+      </c>
       <c r="AI76" s="3"/>
       <c r="AJ76" s="3"/>
     </row>
     <row r="77" spans="1:36">
       <c r="A77" s="0">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3"/>
-      <c r="C77" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -5096,12 +5186,14 @@
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
+      <c r="P77" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="Q77" s="3"/>
-      <c r="R77" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="T77" s="3"/>
       <c r="U77" s="3"/>
       <c r="V77" s="3"/>
@@ -5114,27 +5206,27 @@
       <c r="AC77" s="3"/>
       <c r="AD77" s="3"/>
       <c r="AE77" s="3"/>
-      <c r="AF77" s="3">
-        <v>76</v>
-      </c>
-      <c r="AG77" s="3">
-        <v>74</v>
-      </c>
-      <c r="AH77" s="3">
-        <v>80</v>
-      </c>
+      <c r="AF77" s="3"/>
+      <c r="AG77" s="3"/>
+      <c r="AH77" s="3"/>
       <c r="AI77" s="3"/>
       <c r="AJ77" s="3"/>
     </row>
     <row r="78" spans="1:36">
       <c r="A78" s="0">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -5144,14 +5236,12 @@
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
-      <c r="P78" s="3" t="s">
-        <v>157</v>
-      </c>
+      <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
-      <c r="R78" s="3"/>
-      <c r="S78" s="3" t="s">
-        <v>157</v>
-      </c>
+      <c r="R78" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S78" s="3"/>
       <c r="T78" s="3"/>
       <c r="U78" s="3"/>
       <c r="V78" s="3"/>
@@ -5164,27 +5254,27 @@
       <c r="AC78" s="3"/>
       <c r="AD78" s="3"/>
       <c r="AE78" s="3"/>
-      <c r="AF78" s="3"/>
-      <c r="AG78" s="3"/>
-      <c r="AH78" s="3"/>
+      <c r="AF78" s="3">
+        <v>78</v>
+      </c>
+      <c r="AG78" s="3">
+        <v>74</v>
+      </c>
+      <c r="AH78" s="3">
+        <v>80</v>
+      </c>
       <c r="AI78" s="3"/>
       <c r="AJ78" s="3"/>
     </row>
     <row r="79" spans="1:36">
       <c r="A79" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3"/>
-      <c r="C79" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -5196,10 +5286,10 @@
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
       <c r="Q79" s="3"/>
-      <c r="R79" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
@@ -5212,21 +5302,15 @@
       <c r="AC79" s="3"/>
       <c r="AD79" s="3"/>
       <c r="AE79" s="3"/>
-      <c r="AF79" s="3">
-        <v>78</v>
-      </c>
-      <c r="AG79" s="3">
-        <v>74</v>
-      </c>
-      <c r="AH79" s="3">
-        <v>80</v>
-      </c>
+      <c r="AF79" s="3"/>
+      <c r="AG79" s="3"/>
+      <c r="AH79" s="3"/>
       <c r="AI79" s="3"/>
       <c r="AJ79" s="3"/>
     </row>
     <row r="80" spans="1:36">
       <c r="A80" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5238,15 +5322,23 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
+      <c r="L80" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M80" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
+      <c r="O80" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="P80" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
       <c r="S80" s="3" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
@@ -5268,7 +5360,7 @@
     </row>
     <row r="81" spans="1:36">
       <c r="A81" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5281,22 +5373,20 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="N81" s="3"/>
-      <c r="O81" s="3" t="s">
-        <v>158</v>
-      </c>
+      <c r="O81" s="3"/>
       <c r="P81" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
       <c r="S81" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="T81" s="3"/>
       <c r="U81" s="3"/>
@@ -5318,7 +5408,7 @@
     </row>
     <row r="82" spans="1:36">
       <c r="A82" s="0">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5331,20 +5421,22 @@
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="N82" s="3"/>
-      <c r="O82" s="3"/>
+      <c r="O82" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="P82" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
       <c r="S82" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="T82" s="3"/>
       <c r="U82" s="3"/>
@@ -5366,113 +5458,63 @@
     </row>
     <row r="83" spans="1:36">
       <c r="A83" s="0">
-        <v>81</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
+        <v>82</v>
+      </c>
       <c r="L83" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="N83" s="3"/>
+        <v>161</v>
+      </c>
       <c r="O83" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="3"/>
+        <v>161</v>
+      </c>
       <c r="S83" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="T83" s="3"/>
-      <c r="U83" s="3"/>
-      <c r="V83" s="3"/>
-      <c r="W83" s="3"/>
-      <c r="X83" s="3"/>
-      <c r="Y83" s="3"/>
-      <c r="Z83" s="3"/>
-      <c r="AA83" s="3"/>
-      <c r="AB83" s="3"/>
-      <c r="AC83" s="3"/>
-      <c r="AD83" s="3"/>
-      <c r="AE83" s="3"/>
-      <c r="AF83" s="3"/>
-      <c r="AG83" s="3"/>
-      <c r="AH83" s="3"/>
-      <c r="AI83" s="3"/>
-      <c r="AJ83" s="3"/>
+        <v>161</v>
+      </c>
     </row>
     <row r="84" spans="1:36">
       <c r="A84" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P84" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:36">
       <c r="A85" s="0">
-        <v>83</v>
-      </c>
-      <c r="L85" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M85" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="O85" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="P85" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="S85" s="3" t="s">
-        <v>162</v>
+        <v>84</v>
+      </c>
+      <c r="L85" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="P85" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="S85" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:36">
       <c r="A86" s="0">
-        <v>84</v>
-      </c>
-      <c r="L86" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="P86" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="S86" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="87" spans="1:36">
-      <c r="A87" s="0">
         <v>85</v>
       </c>
-      <c r="V87" s="0" t="s">
+      <c r="V86" s="0" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Syn +goto table +binary search *token number error
</commit_message>
<xml_diff>
--- a/SyntaxAnalyzer/table.xlsx
+++ b/SyntaxAnalyzer/table.xlsx
@@ -1514,9 +1514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
+    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -4550,7 +4550,9 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>

</xml_diff>